<commit_message>
changes in the species translation template
</commit_message>
<xml_diff>
--- a/wildlife_species_list_template.xlsx
+++ b/wildlife_species_list_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wcs1-my.sharepoint.com/personal/dmontecino_wcs_org/Documents/SMART/SMART_WILDLIFE_HEALTH/SMARTeR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{B1CCD1E2-69F5-9544-91BB-490D8563AB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5339BC84-8F19-F544-97AA-D0D28FAC014F}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{B1CCD1E2-69F5-9544-91BB-490D8563AB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAED13AD-7499-7240-809B-52720714D943}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20900" activeTab="3" xr2:uid="{E4DA1E8C-6BE1-40FA-A2B3-614A8BE1E313}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20900" activeTab="1" xr2:uid="{E4DA1E8C-6BE1-40FA-A2B3-614A8BE1E313}"/>
   </bookViews>
   <sheets>
     <sheet name="Mammalia" sheetId="1" r:id="rId1"/>
@@ -1107,9 +1107,6 @@
     <t>ນົກຍາງນ້ອຍ</t>
   </si>
   <si>
-    <t>(blank)</t>
-  </si>
-  <si>
     <t>Woodpecker</t>
   </si>
   <si>
@@ -1450,6 +1447,9 @@
   </si>
   <si>
     <t>common_name_translated</t>
+  </si>
+  <si>
+    <t>Piciformes</t>
   </si>
 </sst>
 </file>
@@ -1626,25 +1626,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1685,6 +1685,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2003,26 +2007,26 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="40.25" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>465</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="16" t="s">
-        <v>460</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -2036,8 +2040,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -2049,8 +2053,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
@@ -2062,8 +2066,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
@@ -2075,8 +2079,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
@@ -2088,8 +2092,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
@@ -2101,8 +2105,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
@@ -2114,8 +2118,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
@@ -2127,8 +2131,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
@@ -2140,8 +2144,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
@@ -2153,8 +2157,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="6" t="s">
         <v>31</v>
       </c>
@@ -2166,8 +2170,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="6" t="s">
         <v>34</v>
       </c>
@@ -2179,8 +2183,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="6" t="s">
         <v>37</v>
       </c>
@@ -2192,8 +2196,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="6" t="s">
         <v>40</v>
       </c>
@@ -2205,8 +2209,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="6" t="s">
         <v>43</v>
       </c>
@@ -2218,8 +2222,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
@@ -2231,8 +2235,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="6" t="s">
         <v>49</v>
       </c>
@@ -2244,8 +2248,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="6" t="s">
         <v>52</v>
       </c>
@@ -2257,8 +2261,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="6" t="s">
         <v>55</v>
       </c>
@@ -2270,8 +2274,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="6" t="s">
         <v>58</v>
       </c>
@@ -2283,8 +2287,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="6" t="s">
         <v>61</v>
       </c>
@@ -2296,8 +2300,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="6" t="s">
         <v>64</v>
       </c>
@@ -2309,8 +2313,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="6" t="s">
         <v>67</v>
       </c>
@@ -2322,8 +2326,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="6" t="s">
         <v>70</v>
       </c>
@@ -2335,8 +2339,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="6" t="s">
         <v>73</v>
       </c>
@@ -2348,8 +2352,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="6" t="s">
         <v>76</v>
       </c>
@@ -2361,8 +2365,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="6" t="s">
         <v>79</v>
       </c>
@@ -2374,8 +2378,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="6" t="s">
         <v>82</v>
       </c>
@@ -2387,8 +2391,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="6" t="s">
         <v>85</v>
       </c>
@@ -2400,8 +2404,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="6" t="s">
         <v>88</v>
       </c>
@@ -2413,8 +2417,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="6" t="s">
         <v>91</v>
       </c>
@@ -2426,8 +2430,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="6" t="s">
         <v>94</v>
       </c>
@@ -2439,8 +2443,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="6" t="s">
         <v>97</v>
       </c>
@@ -2452,8 +2456,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="6" t="s">
         <v>100</v>
       </c>
@@ -2465,8 +2469,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="6" t="s">
         <v>103</v>
       </c>
@@ -2478,8 +2482,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="6" t="s">
         <v>106</v>
       </c>
@@ -2491,8 +2495,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="6" t="s">
         <v>109</v>
       </c>
@@ -2504,8 +2508,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="6" t="s">
         <v>112</v>
       </c>
@@ -2517,8 +2521,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="15">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="6" t="s">
         <v>115</v>
       </c>
@@ -2530,8 +2534,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
       <c r="C41" s="6" t="s">
         <v>118</v>
       </c>
@@ -2543,8 +2547,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="15">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="6" t="s">
         <v>121</v>
       </c>
@@ -2556,8 +2560,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="6" t="s">
         <v>124</v>
       </c>
@@ -2569,8 +2573,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="6" t="s">
         <v>127</v>
       </c>
@@ -2582,8 +2586,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="15">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="6" t="s">
         <v>130</v>
       </c>
@@ -2595,8 +2599,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="6" t="s">
         <v>133</v>
       </c>
@@ -2608,8 +2612,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="15">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="6" t="s">
         <v>136</v>
       </c>
@@ -2621,8 +2625,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="15">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="6" t="s">
         <v>139</v>
       </c>
@@ -2634,8 +2638,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="15">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="6" t="s">
         <v>142</v>
       </c>
@@ -2647,8 +2651,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="15">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="6" t="s">
         <v>145</v>
       </c>
@@ -2660,8 +2664,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="15">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
       <c r="C51" s="6" t="s">
         <v>148</v>
       </c>
@@ -2673,8 +2677,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="15">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="6" t="s">
         <v>151</v>
       </c>
@@ -2686,8 +2690,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="15">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="6" t="s">
         <v>154</v>
       </c>
@@ -2699,8 +2703,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
       <c r="C54" s="6" t="s">
         <v>157</v>
       </c>
@@ -2712,8 +2716,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="15">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
       <c r="C55" s="6" t="s">
         <v>160</v>
       </c>
@@ -2725,8 +2729,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="15">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
       <c r="C56" s="6" t="s">
         <v>163</v>
       </c>
@@ -2738,8 +2742,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="15">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
       <c r="C57" s="6" t="s">
         <v>166</v>
       </c>
@@ -2751,8 +2755,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="15">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
       <c r="C58" s="6" t="s">
         <v>169</v>
       </c>
@@ -2764,8 +2768,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="15">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
       <c r="C59" s="6" t="s">
         <v>172</v>
       </c>
@@ -2777,8 +2781,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="15">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
       <c r="C60" s="6" t="s">
         <v>175</v>
       </c>
@@ -2803,8 +2807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E93148-79D2-4340-87C6-C2BAEF909C37}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2816,26 +2820,26 @@
   <sheetData>
     <row r="1" spans="1:5" ht="42.5" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>465</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>179</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -2849,8 +2853,8 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="19"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="10" t="s">
         <v>183</v>
       </c>
@@ -2862,8 +2866,8 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="19"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="10" t="s">
         <v>186</v>
       </c>
@@ -2875,8 +2879,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="10" t="s">
         <v>189</v>
       </c>
@@ -2888,8 +2892,8 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="19"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="10" t="s">
         <v>192</v>
       </c>
@@ -2901,8 +2905,8 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="19"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="10" t="s">
         <v>195</v>
       </c>
@@ -2914,8 +2918,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="17"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="10" t="s">
         <v>198</v>
       </c>
@@ -2927,8 +2931,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="10" t="s">
         <v>201</v>
       </c>
@@ -2940,8 +2944,8 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="19"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="10" t="s">
         <v>204</v>
       </c>
@@ -2953,8 +2957,8 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="19"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="10" t="s">
         <v>207</v>
       </c>
@@ -2966,8 +2970,8 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="19"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="10" t="s">
         <v>210</v>
       </c>
@@ -2979,8 +2983,8 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="19"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="10" t="s">
         <v>213</v>
       </c>
@@ -2992,8 +2996,8 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="19"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="10" t="s">
         <v>216</v>
       </c>
@@ -3005,8 +3009,8 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="19"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="10" t="s">
         <v>219</v>
       </c>
@@ -3018,8 +3022,8 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="19"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="10" t="s">
         <v>222</v>
       </c>
@@ -3031,8 +3035,8 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="19"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="10" t="s">
         <v>225</v>
       </c>
@@ -3044,8 +3048,8 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="19"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="10" t="s">
         <v>228</v>
       </c>
@@ -3057,8 +3061,8 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="19"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="10" t="s">
         <v>231</v>
       </c>
@@ -3070,8 +3074,8 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="19"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="10" t="s">
         <v>234</v>
       </c>
@@ -3083,8 +3087,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="17.75" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="17"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="10" t="s">
         <v>237</v>
       </c>
@@ -3096,8 +3100,8 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="19"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="10" t="s">
         <v>240</v>
       </c>
@@ -3109,8 +3113,8 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="19"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="10" t="s">
         <v>243</v>
       </c>
@@ -3122,8 +3126,8 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="19"/>
-      <c r="B24" s="17"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="10" t="s">
         <v>246</v>
       </c>
@@ -3135,8 +3139,8 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="19"/>
-      <c r="B25" s="17"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="10" t="s">
         <v>249</v>
       </c>
@@ -3148,8 +3152,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" customHeight="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="10" t="s">
         <v>252</v>
       </c>
@@ -3161,8 +3165,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1">
-      <c r="A27" s="19"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="10" t="s">
         <v>255</v>
       </c>
@@ -3174,8 +3178,8 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="19"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="10" t="s">
         <v>258</v>
       </c>
@@ -3187,8 +3191,8 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="19"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="10" t="s">
         <v>261</v>
       </c>
@@ -3200,8 +3204,8 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="19"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="10" t="s">
         <v>264</v>
       </c>
@@ -3213,8 +3217,8 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="19"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="10" t="s">
         <v>267</v>
       </c>
@@ -3226,8 +3230,8 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="19"/>
-      <c r="B32" s="17"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="10" t="s">
         <v>270</v>
       </c>
@@ -3239,8 +3243,8 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="19"/>
-      <c r="B33" s="17"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="10" t="s">
         <v>273</v>
       </c>
@@ -3252,8 +3256,8 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="19"/>
-      <c r="B34" s="17"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="10" t="s">
         <v>276</v>
       </c>
@@ -3265,8 +3269,8 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="19"/>
-      <c r="B35" s="17"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="19"/>
       <c r="C35" s="10" t="s">
         <v>279</v>
       </c>
@@ -3278,8 +3282,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1">
-      <c r="A36" s="19"/>
-      <c r="B36" s="17"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="10" t="s">
         <v>282</v>
       </c>
@@ -3291,8 +3295,8 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="19"/>
-      <c r="B37" s="17"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="10" t="s">
         <v>285</v>
       </c>
@@ -3304,8 +3308,8 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="19"/>
-      <c r="B38" s="17"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="10" t="s">
         <v>288</v>
       </c>
@@ -3317,8 +3321,8 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="19"/>
-      <c r="B39" s="17"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="10" t="s">
         <v>291</v>
       </c>
@@ -3330,8 +3334,8 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="19"/>
-      <c r="B40" s="17"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="10" t="s">
         <v>294</v>
       </c>
@@ -3343,8 +3347,8 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="19"/>
-      <c r="B41" s="17"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="10" t="s">
         <v>297</v>
       </c>
@@ -3356,8 +3360,8 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="19"/>
-      <c r="B42" s="17"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="10" t="s">
         <v>300</v>
       </c>
@@ -3369,8 +3373,8 @@
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="19"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="10" t="s">
         <v>303</v>
       </c>
@@ -3382,8 +3386,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A44" s="19"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="10" t="s">
         <v>306</v>
       </c>
@@ -3395,8 +3399,8 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="19"/>
-      <c r="B45" s="17"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="10" t="s">
         <v>309</v>
       </c>
@@ -3408,8 +3412,8 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="19"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="10" t="s">
         <v>312</v>
       </c>
@@ -3421,8 +3425,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A47" s="19"/>
-      <c r="B47" s="17"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="19"/>
       <c r="C47" s="10" t="s">
         <v>315</v>
       </c>
@@ -3434,8 +3438,8 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="19"/>
-      <c r="B48" s="17"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="19"/>
       <c r="C48" s="10" t="s">
         <v>318</v>
       </c>
@@ -3447,8 +3451,8 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="19"/>
-      <c r="B49" s="17"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="19"/>
       <c r="C49" s="10" t="s">
         <v>321</v>
       </c>
@@ -3460,8 +3464,8 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="19"/>
-      <c r="B50" s="17"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="19"/>
       <c r="C50" s="10" t="s">
         <v>324</v>
       </c>
@@ -3473,8 +3477,8 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="19"/>
-      <c r="B51" s="17"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="19"/>
       <c r="C51" s="10" t="s">
         <v>327</v>
       </c>
@@ -3486,8 +3490,8 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="19"/>
-      <c r="B52" s="17"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="19"/>
       <c r="C52" s="10" t="s">
         <v>330</v>
       </c>
@@ -3499,8 +3503,8 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="19"/>
-      <c r="B53" s="17"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="19"/>
       <c r="C53" s="10" t="s">
         <v>333</v>
       </c>
@@ -3512,8 +3516,8 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="19"/>
-      <c r="B54" s="17"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="19"/>
       <c r="C54" s="10" t="s">
         <v>336</v>
       </c>
@@ -3525,8 +3529,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="18" customHeight="1">
-      <c r="A55" s="19"/>
-      <c r="B55" s="17"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="19"/>
       <c r="C55" s="10" t="s">
         <v>339</v>
       </c>
@@ -3538,8 +3542,8 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="19"/>
-      <c r="B56" s="17"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="19"/>
       <c r="C56" s="10" t="s">
         <v>342</v>
       </c>
@@ -3551,8 +3555,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A57" s="19"/>
-      <c r="B57" s="17"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="19"/>
       <c r="C57" s="10" t="s">
         <v>345</v>
       </c>
@@ -3564,8 +3568,8 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="19"/>
-      <c r="B58" s="17"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="19"/>
       <c r="C58" s="10" t="s">
         <v>348</v>
       </c>
@@ -3577,198 +3581,198 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A59" s="19"/>
-      <c r="B59" s="17"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="19"/>
       <c r="C59" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="D59" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="E59" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="E59" s="7" t="s">
+    </row>
+    <row r="60" spans="1:5" ht="21" customHeight="1">
+      <c r="A60" s="17"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="10" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="21" customHeight="1">
-      <c r="A60" s="19"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="10" t="s">
+      <c r="D60" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="E60" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="E60" s="7" t="s">
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="17"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="10" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="19"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="10" t="s">
+      <c r="D61" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="E61" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="E61" s="7" t="s">
+    </row>
+    <row r="62" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A62" s="17"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="10" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A62" s="19"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="10" t="s">
+      <c r="D62" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="E62" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="E62" s="7" t="s">
+    </row>
+    <row r="63" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A63" s="17"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="10" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A63" s="19"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="10" t="s">
+      <c r="D63" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="E63" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="E63" s="7" t="s">
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="17"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="10" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="19"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="10" t="s">
+      <c r="D64" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="E64" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="E64" s="7" t="s">
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="17"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="10" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="19"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="10" t="s">
+      <c r="D65" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="E65" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="E65" s="7" t="s">
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="17"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="10" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="19"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="10" t="s">
+      <c r="D66" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="E66" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="E66" s="7" t="s">
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="17"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="10" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="19"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="10" t="s">
+      <c r="D67" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="E67" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="E67" s="7" t="s">
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="17"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="10" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="19"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="10" t="s">
+      <c r="D68" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="D68" s="10" t="s">
+      <c r="E68" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="E68" s="7" t="s">
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="17"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="10" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="19"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="10" t="s">
+      <c r="D69" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="E69" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="E69" s="7" t="s">
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="17"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="10" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="19"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="10" t="s">
+      <c r="D70" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="E70" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="E70" s="7" t="s">
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="17"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="10" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="19"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="10" t="s">
+      <c r="D71" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="D71" s="10" t="s">
+      <c r="E71" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="E71" s="7" t="s">
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="17"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="10" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="19"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="10" t="s">
+      <c r="D72" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="D72" s="10" t="s">
+      <c r="E72" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="E72" s="7" t="s">
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="18"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="10" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="20"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="10" t="s">
+      <c r="D73" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="D73" s="10" t="s">
+      <c r="E73" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -3776,8 +3780,11 @@
     <mergeCell ref="A2:A73"/>
     <mergeCell ref="B2:B73"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C59" r:id="rId1" display="https://www.google.com/search?rlz=1C5CHFA_enUS916US917&amp;q=Piciformes&amp;stick=H4sIAAAAAAAAAONgVuLUz9U3MMzKzipYxMoVkJmcmZZflJtaDAC8IEdbGgAAAA&amp;sa=X&amp;ved=2ahUKEwjlmI6Wpcj_AhVBBNQKHYJCDG4QmxMoAXoECDkQAw" xr:uid="{D324789D-F048-E549-9171-822072B4A5AD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3799,270 +3806,270 @@
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>465</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>396</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="E2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="7" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="E3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="7" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="E4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="7" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="E5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="7" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="E6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="7" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="E7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="7" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="E8" s="7" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="7" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="E9" s="7" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="7" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="E10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="7" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="E11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="7" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="E12" s="7" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="7" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="E13" s="7" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="7" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="E14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="7" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="E15" s="7" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="7" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="E16" s="7" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="7" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="E17" s="7" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="7" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="E18" s="7" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="7" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="E19" s="7" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="20.5" customHeight="1">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="7" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="20.5" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>453</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4079,7 +4086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44C46B9-3B51-461D-A385-14C2195E44F2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -4094,36 +4101,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36.5" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>458</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -4142,6 +4149,49 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="084233d8-102a-4822-bcb5-34ef88036187" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6ff2f07d-e36f-484d-8783-7471b0b7cd38">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="084233d8-102a-4822-bcb5-34ef88036187">
+      <UserInfo>
+        <DisplayName>Olson, Sarah</DisplayName>
+        <AccountId>30</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Phouangsouvanh, Souchinda</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Montecino, Diego</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Khammavong, Kongsy</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Denstedt, Emily</DisplayName>
+        <AccountId>6</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Milavong, Phonesavanh</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE607FA88307C54AA0C229525D16D6DD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd7bd6d9291f2d99bdecd3eff25e4c93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ff2f07d-e36f-484d-8783-7471b0b7cd38" xmlns:ns3="084233d8-102a-4822-bcb5-34ef88036187" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="96024ee9f9910ef71bd2f1305740cda4" ns2:_="" ns3:_="">
     <xsd:import namespace="6ff2f07d-e36f-484d-8783-7471b0b7cd38"/>
@@ -4378,49 +4428,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="084233d8-102a-4822-bcb5-34ef88036187" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6ff2f07d-e36f-484d-8783-7471b0b7cd38">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="084233d8-102a-4822-bcb5-34ef88036187">
-      <UserInfo>
-        <DisplayName>Olson, Sarah</DisplayName>
-        <AccountId>30</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Phouangsouvanh, Souchinda</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Montecino, Diego</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Khammavong, Kongsy</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Denstedt, Emily</DisplayName>
-        <AccountId>6</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Milavong, Phonesavanh</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32496430-ED49-4DE8-BE7A-081C6AB1FB4B}">
   <ds:schemaRefs>
@@ -4430,6 +4437,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07568FC2-AE26-475F-8424-B3928827AFB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="084233d8-102a-4822-bcb5-34ef88036187"/>
+    <ds:schemaRef ds:uri="6ff2f07d-e36f-484d-8783-7471b0b7cd38"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55BEAA73-857A-47AB-B45E-087A2BA0A8C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4446,21 +4470,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07568FC2-AE26-475F-8424-B3928827AFB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="084233d8-102a-4822-bcb5-34ef88036187"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6ff2f07d-e36f-484d-8783-7471b0b7cd38"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>